<commit_message>
Implement baseline of file uploading feature
This commit includes setting up the foundation for file uploading functionalities. It also includes added different window management methods, creation of various manager structures and implementing window shifting. Additional error handling cases have been considered by defining new message types. Unit tests have been written to ensure the correct functioning of the written code.
</commit_message>
<xml_diff>
--- a/doc/RRTTP/Packet_Structure.xlsx
+++ b/doc/RRTTP/Packet_Structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ReliableRealTimeTransportProtocol\doc\RRTTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8384640-F036-4718-9733-29B468487503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCDDBAE-38E3-4A43-A993-1B7B04ECAAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DE0CD10-A31D-4036-A1AA-8A58F69C54A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{4DE0CD10-A31D-4036-A1AA-8A58F69C54A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>RES</t>
   </si>
   <si>
-    <t>RESERVED</t>
-  </si>
-  <si>
     <t>Data Offset</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>Data Length</t>
+  </si>
+  <si>
+    <t>Channel ID</t>
   </si>
 </sst>
 </file>
@@ -393,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -404,18 +404,60 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -428,28 +470,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -458,27 +478,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -797,62 +796,62 @@
   <dimension ref="A1:AH9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="K5" sqref="K5:R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="7">
+      <c r="B1" s="19"/>
+      <c r="C1" s="20">
         <v>0</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="7">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="20">
         <v>1</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="7">
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="20">
         <v>2</v>
       </c>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="7">
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="20">
         <v>3</v>
       </c>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="8"/>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="21"/>
+      <c r="AE1" s="21"/>
+      <c r="AF1" s="21"/>
+      <c r="AG1" s="21"/>
+      <c r="AH1" s="22"/>
     </row>
     <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1">
@@ -960,83 +959,83 @@
         <f>A3*8</f>
         <v>0</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="10"/>
-      <c r="AD3" s="10"/>
-      <c r="AE3" s="10"/>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="10"/>
-      <c r="AH3" s="11"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24"/>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="24"/>
+      <c r="AH3" s="25"/>
     </row>
     <row r="4" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ref="B4:B8" si="0">A4*8</f>
+        <f t="shared" ref="B4:B6" si="0">A4*8</f>
         <v>32</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="21"/>
-      <c r="X4" s="21"/>
-      <c r="Y4" s="21"/>
-      <c r="Z4" s="21"/>
-      <c r="AA4" s="21"/>
-      <c r="AB4" s="21"/>
-      <c r="AC4" s="21"/>
-      <c r="AD4" s="21"/>
-      <c r="AE4" s="21"/>
-      <c r="AF4" s="21"/>
-      <c r="AG4" s="21"/>
-      <c r="AH4" s="22"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="27"/>
+      <c r="W4" s="27"/>
+      <c r="X4" s="27"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="27"/>
+      <c r="AA4" s="27"/>
+      <c r="AB4" s="27"/>
+      <c r="AC4" s="27"/>
+      <c r="AD4" s="27"/>
+      <c r="AE4" s="27"/>
+      <c r="AF4" s="27"/>
+      <c r="AG4" s="27"/>
+      <c r="AH4" s="28"/>
     </row>
     <row r="5" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
@@ -1046,60 +1045,60 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" s="26" t="s">
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="T5" s="27"/>
-      <c r="U5" s="27"/>
-      <c r="V5" s="27"/>
-      <c r="W5" s="27"/>
-      <c r="X5" s="27"/>
-      <c r="Y5" s="27"/>
-      <c r="Z5" s="28"/>
-      <c r="AA5" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB5" s="24"/>
-      <c r="AC5" s="24"/>
-      <c r="AD5" s="24"/>
-      <c r="AE5" s="24"/>
-      <c r="AF5" s="24"/>
-      <c r="AG5" s="24"/>
-      <c r="AH5" s="25"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="7"/>
     </row>
     <row r="6" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -1110,7 +1109,7 @@
         <v>96</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -1146,10 +1145,10 @@
     </row>
     <row r="7" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
@@ -1186,13 +1185,13 @@
     </row>
     <row r="8" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -1228,10 +1227,10 @@
     </row>
     <row r="9" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
@@ -1269,18 +1268,18 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="12">
+    <mergeCell ref="C3:AH3"/>
+    <mergeCell ref="C4:AH4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="K1:R1"/>
+    <mergeCell ref="S1:Z1"/>
+    <mergeCell ref="AA1:AH1"/>
     <mergeCell ref="AA5:AH5"/>
     <mergeCell ref="S5:Z5"/>
     <mergeCell ref="K5:R5"/>
     <mergeCell ref="C8:AH9"/>
     <mergeCell ref="C6:AH7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="K1:R1"/>
-    <mergeCell ref="S1:Z1"/>
-    <mergeCell ref="AA1:AH1"/>
-    <mergeCell ref="C3:AH3"/>
-    <mergeCell ref="C4:AH4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactors transport layer, adds window management functionality
The transport layer is refactored while adding window management functionalities as part of the foundational setup for a file uploading feature. New structures such as WindowManager and TransmitterWindow have been created and methods for handling messages and shifting window have been implemented. This update also defines new message types for enhanced error handling. Unit tests are included to ensure the functionality works as expected.
</commit_message>
<xml_diff>
--- a/doc/RRTTP/Packet_Structure.xlsx
+++ b/doc/RRTTP/Packet_Structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ReliableRealTimeTransportProtocol\doc\RRTTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCDDBAE-38E3-4A43-A993-1B7B04ECAAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488C5636-03B9-4070-9761-7436DD19F452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{4DE0CD10-A31D-4036-A1AA-8A58F69C54A6}"/>
+    <workbookView minimized="1" xWindow="4530" yWindow="8820" windowWidth="28800" windowHeight="15435" xr2:uid="{4DE0CD10-A31D-4036-A1AA-8A58F69C54A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Offsets</t>
   </si>
@@ -47,12 +47,6 @@
     <t>Bit</t>
   </si>
   <si>
-    <t>Sequence number</t>
-  </si>
-  <si>
-    <t>Acknowledgment number (if ACK set)</t>
-  </si>
-  <si>
     <t>ACK</t>
   </si>
   <si>
@@ -81,6 +75,9 @@
   </si>
   <si>
     <t>Channel ID</t>
+  </si>
+  <si>
+    <t>Sequence number, Acknowledgment number (if ACK set)</t>
   </si>
 </sst>
 </file>
@@ -143,7 +140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -287,43 +284,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFA2A9B1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFA2A9B1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFA2A9B1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFA2A9B1"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA2A9B1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -393,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -407,25 +367,49 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -444,39 +428,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -793,59 +744,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FCB3819-1452-4A4B-8F96-F86B0B28D25F}">
-  <dimension ref="A1:AH9"/>
+  <dimension ref="A1:AH8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:R5"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20">
+      <c r="B1" s="9"/>
+      <c r="C1" s="10">
         <v>0</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="20">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="10">
         <v>1</v>
       </c>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="20">
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="10">
         <v>2</v>
       </c>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="20">
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="10">
         <v>3</v>
       </c>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="22"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="12"/>
     </row>
     <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -959,327 +910,283 @@
         <f>A3*8</f>
         <v>0</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="7"/>
+    </row>
+    <row r="4" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" ref="B4:B5" si="0">A4*8</f>
+        <v>32</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="24"/>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="24"/>
-      <c r="AD3" s="24"/>
-      <c r="AE3" s="24"/>
-      <c r="AF3" s="24"/>
-      <c r="AG3" s="24"/>
-      <c r="AH3" s="25"/>
+      <c r="K4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="14"/>
+      <c r="AF4" s="14"/>
+      <c r="AG4" s="14"/>
+      <c r="AH4" s="15"/>
     </row>
-    <row r="4" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <f t="shared" ref="B4:B6" si="0">A4*8</f>
-        <v>32</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27"/>
-      <c r="V4" s="27"/>
-      <c r="W4" s="27"/>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
-      <c r="Z4" s="27"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
-      <c r="AE4" s="27"/>
-      <c r="AF4" s="27"/>
-      <c r="AG4" s="27"/>
-      <c r="AH4" s="28"/>
-    </row>
-    <row r="5" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+    <row r="5" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>8</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="9"/>
-      <c r="AA5" s="5" t="s">
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="21"/>
+      <c r="AC5" s="21"/>
+      <c r="AD5" s="21"/>
+      <c r="AE5" s="21"/>
+      <c r="AF5" s="21"/>
+      <c r="AG5" s="21"/>
+      <c r="AH5" s="22"/>
+    </row>
+    <row r="6" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="6"/>
-      <c r="AG5" s="6"/>
-      <c r="AH5" s="7"/>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="24"/>
+      <c r="AA6" s="24"/>
+      <c r="AB6" s="24"/>
+      <c r="AC6" s="24"/>
+      <c r="AD6" s="24"/>
+      <c r="AE6" s="24"/>
+      <c r="AF6" s="24"/>
+      <c r="AG6" s="24"/>
+      <c r="AH6" s="25"/>
     </row>
-    <row r="6" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2">
-        <f t="shared" si="0"/>
-        <v>96</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="13"/>
-      <c r="AD6" s="13"/>
-      <c r="AE6" s="13"/>
-      <c r="AF6" s="13"/>
-      <c r="AG6" s="13"/>
-      <c r="AH6" s="14"/>
-    </row>
-    <row r="7" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="16"/>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="16"/>
-      <c r="AB7" s="16"/>
-      <c r="AC7" s="16"/>
-      <c r="AD7" s="16"/>
-      <c r="AE7" s="16"/>
-      <c r="AF7" s="16"/>
-      <c r="AG7" s="16"/>
-      <c r="AH7" s="17"/>
+      <c r="C7" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="21"/>
+      <c r="Z7" s="21"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="21"/>
+      <c r="AC7" s="21"/>
+      <c r="AD7" s="21"/>
+      <c r="AE7" s="21"/>
+      <c r="AF7" s="21"/>
+      <c r="AG7" s="21"/>
+      <c r="AH7" s="22"/>
     </row>
-    <row r="8" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="13"/>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="13"/>
-      <c r="AD8" s="13"/>
-      <c r="AE8" s="13"/>
-      <c r="AF8" s="13"/>
-      <c r="AG8" s="13"/>
-      <c r="AH8" s="14"/>
-    </row>
-    <row r="9" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="16"/>
-      <c r="AA9" s="16"/>
-      <c r="AB9" s="16"/>
-      <c r="AC9" s="16"/>
-      <c r="AD9" s="16"/>
-      <c r="AE9" s="16"/>
-      <c r="AF9" s="16"/>
-      <c r="AG9" s="16"/>
-      <c r="AH9" s="17"/>
+        <v>7</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="24"/>
+      <c r="AB8" s="24"/>
+      <c r="AC8" s="24"/>
+      <c r="AD8" s="24"/>
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="24"/>
+      <c r="AG8" s="24"/>
+      <c r="AH8" s="25"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="12">
+  <mergeCells count="11">
+    <mergeCell ref="AA4:AH4"/>
+    <mergeCell ref="S4:Z4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="C7:AH8"/>
+    <mergeCell ref="C5:AH6"/>
     <mergeCell ref="C3:AH3"/>
-    <mergeCell ref="C4:AH4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="K1:R1"/>
     <mergeCell ref="S1:Z1"/>
     <mergeCell ref="AA1:AH1"/>
-    <mergeCell ref="AA5:AH5"/>
-    <mergeCell ref="S5:Z5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="C8:AH9"/>
-    <mergeCell ref="C6:AH7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update window management in transport layer
Modified the transport layer by incorporating window management functions to enhance file uploading feature. Includes the creation of WindowManager and TransmitterWindow structures, implementation of message handling methods and shifting windows, the introduction of new message types for improved error handling, and unit tests for validation.
</commit_message>
<xml_diff>
--- a/doc/RRTTP/Packet_Structure.xlsx
+++ b/doc/RRTTP/Packet_Structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ReliableRealTimeTransportProtocol\doc\RRTTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488C5636-03B9-4070-9761-7436DD19F452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F2704A-B0FD-45A4-BA31-C2FE44F4A767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4530" yWindow="8820" windowWidth="28800" windowHeight="15435" xr2:uid="{4DE0CD10-A31D-4036-A1AA-8A58F69C54A6}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DE0CD10-A31D-4036-A1AA-8A58F69C54A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Offsets</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Sequence number, Acknowledgment number (if ACK set)</t>
+  </si>
+  <si>
+    <t>Reserved</t>
   </si>
 </sst>
 </file>
@@ -367,6 +370,45 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -390,45 +432,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -744,59 +747,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FCB3819-1452-4A4B-8F96-F86B0B28D25F}">
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:AH9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23">
         <v>0</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="10">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="23">
         <v>1</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="10">
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="23">
         <v>2</v>
       </c>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="10">
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="23">
         <v>3</v>
       </c>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
-      <c r="AG1" s="11"/>
-      <c r="AH1" s="12"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="25"/>
     </row>
     <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -902,7 +905,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -910,283 +913,327 @@
         <f>A3*8</f>
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="6"/>
-      <c r="AH3" s="7"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="19"/>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="19"/>
+      <c r="AB3" s="19"/>
+      <c r="AC3" s="19"/>
+      <c r="AD3" s="19"/>
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="19"/>
+      <c r="AG3" s="19"/>
+      <c r="AH3" s="20"/>
     </row>
-    <row r="4" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+    <row r="4" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ref="B4:B5" si="0">A4*8</f>
+        <f>A4*8</f>
         <v>32</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="19"/>
+      <c r="AE4" s="19"/>
+      <c r="AF4" s="19"/>
+      <c r="AG4" s="19"/>
+      <c r="AH4" s="20"/>
+    </row>
+    <row r="5" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" ref="B5:B6" si="0">A5*8</f>
+        <v>64</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="7"/>
+    </row>
+    <row r="6" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>12</v>
       </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="17"/>
-      <c r="AA4" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB4" s="14"/>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
-      <c r="AE4" s="14"/>
-      <c r="AF4" s="14"/>
-      <c r="AG4" s="14"/>
-      <c r="AH4" s="15"/>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13"/>
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="14"/>
     </row>
-    <row r="5" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+    <row r="7" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="16"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7" s="16"/>
+      <c r="AF7" s="16"/>
+      <c r="AG7" s="16"/>
+      <c r="AH7" s="17"/>
+    </row>
+    <row r="8" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21"/>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="21"/>
-      <c r="AC5" s="21"/>
-      <c r="AD5" s="21"/>
-      <c r="AE5" s="21"/>
-      <c r="AF5" s="21"/>
-      <c r="AG5" s="21"/>
-      <c r="AH5" s="22"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="13"/>
+      <c r="AD8" s="13"/>
+      <c r="AE8" s="13"/>
+      <c r="AF8" s="13"/>
+      <c r="AG8" s="13"/>
+      <c r="AH8" s="14"/>
     </row>
-    <row r="6" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="9" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24"/>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="24"/>
-      <c r="AB6" s="24"/>
-      <c r="AC6" s="24"/>
-      <c r="AD6" s="24"/>
-      <c r="AE6" s="24"/>
-      <c r="AF6" s="24"/>
-      <c r="AG6" s="24"/>
-      <c r="AH6" s="25"/>
-    </row>
-    <row r="7" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
-      <c r="AA7" s="21"/>
-      <c r="AB7" s="21"/>
-      <c r="AC7" s="21"/>
-      <c r="AD7" s="21"/>
-      <c r="AE7" s="21"/>
-      <c r="AF7" s="21"/>
-      <c r="AG7" s="21"/>
-      <c r="AH7" s="22"/>
-    </row>
-    <row r="8" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="24"/>
-      <c r="AA8" s="24"/>
-      <c r="AB8" s="24"/>
-      <c r="AC8" s="24"/>
-      <c r="AD8" s="24"/>
-      <c r="AE8" s="24"/>
-      <c r="AF8" s="24"/>
-      <c r="AG8" s="24"/>
-      <c r="AH8" s="25"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="16"/>
+      <c r="X9" s="16"/>
+      <c r="Y9" s="16"/>
+      <c r="Z9" s="16"/>
+      <c r="AA9" s="16"/>
+      <c r="AB9" s="16"/>
+      <c r="AC9" s="16"/>
+      <c r="AD9" s="16"/>
+      <c r="AE9" s="16"/>
+      <c r="AF9" s="16"/>
+      <c r="AG9" s="16"/>
+      <c r="AH9" s="17"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="11">
-    <mergeCell ref="AA4:AH4"/>
-    <mergeCell ref="S4:Z4"/>
-    <mergeCell ref="K4:R4"/>
-    <mergeCell ref="C7:AH8"/>
-    <mergeCell ref="C5:AH6"/>
-    <mergeCell ref="C3:AH3"/>
+  <mergeCells count="12">
+    <mergeCell ref="C4:AH4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="K1:R1"/>
     <mergeCell ref="S1:Z1"/>
     <mergeCell ref="AA1:AH1"/>
+    <mergeCell ref="C3:AH3"/>
+    <mergeCell ref="AA5:AH5"/>
+    <mergeCell ref="S5:Z5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="C8:AH9"/>
+    <mergeCell ref="C6:AH7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Remove numerous files and modify existing code in transport layer
Deleted several files related to connection management, window management and transmission in the transport layer, as part of a refactoring process to streamline and simplify the existing codebase. Modifications were made accordingly to the remaining files, mainly `window.rs` and `transport_layer.rs`, to ensure smooth functioning of the layer, removing redundancies and decreasing overall complexity.
</commit_message>
<xml_diff>
--- a/doc/RRTTP/Packet_Structure.xlsx
+++ b/doc/RRTTP/Packet_Structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ReliableRealTimeTransportProtocol\doc\RRTTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F2704A-B0FD-45A4-BA31-C2FE44F4A767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5016538D-8D5D-440B-BA6E-64A44527CE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DE0CD10-A31D-4036-A1AA-8A58F69C54A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{4DE0CD10-A31D-4036-A1AA-8A58F69C54A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Offsets</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Data Length</t>
-  </si>
-  <si>
-    <t>Channel ID</t>
   </si>
   <si>
     <t>Sequence number, Acknowledgment number (if ACK set)</t>
@@ -370,6 +367,30 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -408,30 +429,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -747,59 +744,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FCB3819-1452-4A4B-8F96-F86B0B28D25F}">
-  <dimension ref="A1:AH9"/>
+  <dimension ref="A1:AH8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="C7" sqref="C7:AH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="23">
+      <c r="B1" s="9"/>
+      <c r="C1" s="10">
         <v>0</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="23">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="10">
         <v>1</v>
       </c>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="23">
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="10">
         <v>2</v>
       </c>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="23">
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="10">
         <v>3</v>
       </c>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="25"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="12"/>
     </row>
     <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -913,327 +910,283 @@
         <f>A3*8</f>
         <v>0</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="7"/>
+    </row>
+    <row r="4" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" ref="B4:B5" si="0">A4*8</f>
+        <v>32</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="19"/>
-      <c r="V3" s="19"/>
-      <c r="W3" s="19"/>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="19"/>
-      <c r="Z3" s="19"/>
-      <c r="AA3" s="19"/>
-      <c r="AB3" s="19"/>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="19"/>
-      <c r="AE3" s="19"/>
-      <c r="AF3" s="19"/>
-      <c r="AG3" s="19"/>
-      <c r="AH3" s="20"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="14"/>
+      <c r="AF4" s="14"/>
+      <c r="AG4" s="14"/>
+      <c r="AH4" s="15"/>
     </row>
-    <row r="4" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <f>A4*8</f>
-        <v>32</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="19"/>
-      <c r="X4" s="19"/>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="19"/>
-      <c r="AA4" s="19"/>
-      <c r="AB4" s="19"/>
-      <c r="AC4" s="19"/>
-      <c r="AD4" s="19"/>
-      <c r="AE4" s="19"/>
-      <c r="AF4" s="19"/>
-      <c r="AG4" s="19"/>
-      <c r="AH4" s="20"/>
+    <row r="5" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="21"/>
+      <c r="AC5" s="21"/>
+      <c r="AD5" s="21"/>
+      <c r="AE5" s="21"/>
+      <c r="AF5" s="21"/>
+      <c r="AG5" s="21"/>
+      <c r="AH5" s="22"/>
     </row>
-    <row r="5" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+    <row r="6" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="24"/>
+      <c r="AA6" s="24"/>
+      <c r="AB6" s="24"/>
+      <c r="AC6" s="24"/>
+      <c r="AD6" s="24"/>
+      <c r="AE6" s="24"/>
+      <c r="AF6" s="24"/>
+      <c r="AG6" s="24"/>
+      <c r="AH6" s="25"/>
+    </row>
+    <row r="7" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
-        <f t="shared" ref="B5:B6" si="0">A5*8</f>
-        <v>64</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="9"/>
-      <c r="AA5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="6"/>
-      <c r="AG5" s="6"/>
-      <c r="AH5" s="7"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="21"/>
+      <c r="Z7" s="21"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="21"/>
+      <c r="AC7" s="21"/>
+      <c r="AD7" s="21"/>
+      <c r="AE7" s="21"/>
+      <c r="AF7" s="21"/>
+      <c r="AG7" s="21"/>
+      <c r="AH7" s="22"/>
     </row>
-    <row r="6" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2">
-        <f t="shared" si="0"/>
-        <v>96</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="13"/>
-      <c r="AD6" s="13"/>
-      <c r="AE6" s="13"/>
-      <c r="AF6" s="13"/>
-      <c r="AG6" s="13"/>
-      <c r="AH6" s="14"/>
-    </row>
-    <row r="7" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="16"/>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="16"/>
-      <c r="AB7" s="16"/>
-      <c r="AC7" s="16"/>
-      <c r="AD7" s="16"/>
-      <c r="AE7" s="16"/>
-      <c r="AF7" s="16"/>
-      <c r="AG7" s="16"/>
-      <c r="AH7" s="17"/>
-    </row>
-    <row r="8" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="13"/>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="13"/>
-      <c r="AD8" s="13"/>
-      <c r="AE8" s="13"/>
-      <c r="AF8" s="13"/>
-      <c r="AG8" s="13"/>
-      <c r="AH8" s="14"/>
-    </row>
-    <row r="9" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="16"/>
-      <c r="AA9" s="16"/>
-      <c r="AB9" s="16"/>
-      <c r="AC9" s="16"/>
-      <c r="AD9" s="16"/>
-      <c r="AE9" s="16"/>
-      <c r="AF9" s="16"/>
-      <c r="AG9" s="16"/>
-      <c r="AH9" s="17"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="24"/>
+      <c r="AB8" s="24"/>
+      <c r="AC8" s="24"/>
+      <c r="AD8" s="24"/>
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="24"/>
+      <c r="AG8" s="24"/>
+      <c r="AH8" s="25"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="12">
-    <mergeCell ref="C4:AH4"/>
+  <mergeCells count="11">
+    <mergeCell ref="AA4:AH4"/>
+    <mergeCell ref="S4:Z4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="C7:AH8"/>
+    <mergeCell ref="C5:AH6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="K1:R1"/>
     <mergeCell ref="S1:Z1"/>
     <mergeCell ref="AA1:AH1"/>
     <mergeCell ref="C3:AH3"/>
-    <mergeCell ref="AA5:AH5"/>
-    <mergeCell ref="S5:Z5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="C8:AH9"/>
-    <mergeCell ref="C6:AH7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add debugging configurations and updates file processing logic
This commit introduces new run configurations for ease in debugging. It also includes changes in the processing logic in connection_processor.rs and the transmitter_window.rs files that involve handling received and sent data. Additionally, the update includes modifications to the log message and rust type definition files, where the 'FileRejected' and 'FileAccepted' definitions now include NetworkFileInfo.
</commit_message>
<xml_diff>
--- a/doc/RRTTP/Packet_Structure.xlsx
+++ b/doc/RRTTP/Packet_Structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ReliableRealTimeTransportProtocol\doc\RRTTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5016538D-8D5D-440B-BA6E-64A44527CE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5166B47-9013-4334-B0EF-1EEB1DC22AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{4DE0CD10-A31D-4036-A1AA-8A58F69C54A6}"/>
+    <workbookView minimized="1" xWindow="38400" yWindow="45" windowWidth="28800" windowHeight="15435" xr2:uid="{4DE0CD10-A31D-4036-A1AA-8A58F69C54A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -367,6 +367,60 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -374,60 +428,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -448,9 +448,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -488,7 +488,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -594,7 +594,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -736,7 +736,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -746,57 +746,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FCB3819-1452-4A4B-8F96-F86B0B28D25F}">
   <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C7" sqref="C7:AH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10">
+      <c r="B1" s="19"/>
+      <c r="C1" s="20">
         <v>0</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="10">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="20">
         <v>1</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="10">
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="20">
         <v>2</v>
       </c>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="10">
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="20">
         <v>3</v>
       </c>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
-      <c r="AG1" s="11"/>
-      <c r="AH1" s="12"/>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="21"/>
+      <c r="AE1" s="21"/>
+      <c r="AF1" s="21"/>
+      <c r="AG1" s="21"/>
+      <c r="AH1" s="22"/>
     </row>
     <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -910,40 +910,40 @@
         <f>A3*8</f>
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="6"/>
-      <c r="AH3" s="7"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24"/>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="24"/>
+      <c r="AH3" s="25"/>
     </row>
     <row r="4" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
@@ -977,36 +977,36 @@
       <c r="J4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="16" t="s">
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="17"/>
-      <c r="AA4" s="13" t="s">
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AB4" s="14"/>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
-      <c r="AE4" s="14"/>
-      <c r="AF4" s="14"/>
-      <c r="AG4" s="14"/>
-      <c r="AH4" s="15"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="7"/>
     </row>
     <row r="5" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -1016,40 +1016,40 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21"/>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="21"/>
-      <c r="AC5" s="21"/>
-      <c r="AD5" s="21"/>
-      <c r="AE5" s="21"/>
-      <c r="AF5" s="21"/>
-      <c r="AG5" s="21"/>
-      <c r="AH5" s="22"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="13"/>
+      <c r="AF5" s="13"/>
+      <c r="AG5" s="13"/>
+      <c r="AH5" s="14"/>
     </row>
     <row r="6" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -1058,38 +1058,38 @@
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24"/>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="24"/>
-      <c r="AB6" s="24"/>
-      <c r="AC6" s="24"/>
-      <c r="AD6" s="24"/>
-      <c r="AE6" s="24"/>
-      <c r="AF6" s="24"/>
-      <c r="AG6" s="24"/>
-      <c r="AH6" s="25"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="16"/>
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="16"/>
+      <c r="AF6" s="16"/>
+      <c r="AG6" s="16"/>
+      <c r="AH6" s="17"/>
     </row>
     <row r="7" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1098,40 +1098,40 @@
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
-      <c r="AA7" s="21"/>
-      <c r="AB7" s="21"/>
-      <c r="AC7" s="21"/>
-      <c r="AD7" s="21"/>
-      <c r="AE7" s="21"/>
-      <c r="AF7" s="21"/>
-      <c r="AG7" s="21"/>
-      <c r="AH7" s="22"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="13"/>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13"/>
+      <c r="AE7" s="13"/>
+      <c r="AF7" s="13"/>
+      <c r="AG7" s="13"/>
+      <c r="AH7" s="14"/>
     </row>
     <row r="8" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -1140,53 +1140,53 @@
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="24"/>
-      <c r="AA8" s="24"/>
-      <c r="AB8" s="24"/>
-      <c r="AC8" s="24"/>
-      <c r="AD8" s="24"/>
-      <c r="AE8" s="24"/>
-      <c r="AF8" s="24"/>
-      <c r="AG8" s="24"/>
-      <c r="AH8" s="25"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="16"/>
+      <c r="Z8" s="16"/>
+      <c r="AA8" s="16"/>
+      <c r="AB8" s="16"/>
+      <c r="AC8" s="16"/>
+      <c r="AD8" s="16"/>
+      <c r="AE8" s="16"/>
+      <c r="AF8" s="16"/>
+      <c r="AG8" s="16"/>
+      <c r="AH8" s="17"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="11">
+    <mergeCell ref="C3:AH3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="K1:R1"/>
+    <mergeCell ref="S1:Z1"/>
+    <mergeCell ref="AA1:AH1"/>
     <mergeCell ref="AA4:AH4"/>
     <mergeCell ref="S4:Z4"/>
     <mergeCell ref="K4:R4"/>
     <mergeCell ref="C7:AH8"/>
     <mergeCell ref="C5:AH6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="K1:R1"/>
-    <mergeCell ref="S1:Z1"/>
-    <mergeCell ref="AA1:AH1"/>
-    <mergeCell ref="C3:AH3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>